<commit_message>
Add Azure dependencies and start sending messages
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\lnu\internet_architectures\swms-device-simulator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69C4525-9488-446D-BBA9-A65D53708D19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E898090-2668-4A9E-B354-9253722FE941}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E2AC1783-8C2A-498D-AE30-0E6C43A8A69B}"/>
   </bookViews>
@@ -32,6 +32,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>HostName=filipiothub.azure-devices.net;DeviceId=bin-008;SharedAccessKey=Jm/zGBgY1ddtbRXaL9miMwi8zX/mHGMyBp1N8R4ZSYg=</t>
+  </si>
+  <si>
+    <t>HostName=filipiothub.azure-devices.net;DeviceId=bin-006;SharedAccessKey=aNPACA6knFTNhaH5SN/WTsFh+Q6xF272WtJYef6RN2s=</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,28 +394,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9894CE4-21DD-41EB-92EB-886AF8878013}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -415,7 +420,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -426,10 +431,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -437,10 +442,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -448,10 +453,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
-        <v>14.5</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -459,10 +464,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
-        <v>20</v>
+        <v>14.5</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -470,10 +475,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
-        <v>26.05</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -481,10 +486,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1">
-        <v>32</v>
+        <v>26.05</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -492,10 +497,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -503,10 +508,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -514,10 +519,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -525,10 +530,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -536,10 +541,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -547,10 +552,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -558,10 +563,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -569,10 +574,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -580,10 +585,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -591,10 +596,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -602,19 +607,25 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
+        <v>89</v>
+      </c>
+      <c r="B20" s="1">
+        <v>92</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1">
         <v>94</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>98</v>
       </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1"/>
@@ -640,6 +651,11 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -649,28 +665,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620C1B83-CAB1-4591-B467-7BE45F763CB8}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -681,7 +691,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -692,10 +702,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -703,10 +713,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -714,10 +724,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
-        <v>12</v>
+        <v>9.5</v>
       </c>
       <c r="B6" s="1">
-        <v>14.5</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -725,10 +735,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
         <v>14.5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>20</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -736,10 +746,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
-        <v>17</v>
+        <v>14.5</v>
       </c>
       <c r="B8" s="1">
-        <v>26.05</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -747,10 +757,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
-        <v>19.5</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
-        <v>32</v>
+        <v>26.05</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -758,10 +768,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
-        <v>22</v>
+        <v>19.5</v>
       </c>
       <c r="B10" s="1">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -769,10 +779,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
-        <v>24.5</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -780,10 +790,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
-        <v>27</v>
+        <v>24.5</v>
       </c>
       <c r="B12" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -791,10 +801,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -802,10 +812,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
-        <v>32</v>
+        <v>29.5</v>
       </c>
       <c r="B14" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -813,10 +823,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
-        <v>34.5</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -824,10 +834,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
-        <v>37</v>
+        <v>34.5</v>
       </c>
       <c r="B16" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -835,10 +845,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
-        <v>39.5</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -846,10 +856,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
-        <v>42</v>
+        <v>39.5</v>
       </c>
       <c r="B18" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -857,10 +867,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
-        <v>44.5</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -868,19 +878,25 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
+        <v>44.5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1">
         <v>47</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>24.5</v>
       </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1"/>
@@ -907,6 +923,11 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>